<commit_message>
not working when loading
</commit_message>
<xml_diff>
--- a/backend/training/glossing/data/cleaned_inspection.xlsx
+++ b/backend/training/glossing/data/cleaned_inspection.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,240 +448,420 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>der den keks isst</t>
+          <t>der Keksessende</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DEM.M.SG.NOM ART.DEF.M.SG.ACC cookie.M.SG.ACC eat\PRS-.SG.IND</t>
+          <t>the.ART.DEF.M.SG.NOM biscuit-end.M.SG.NOM</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>der hingefallen ist</t>
+          <t>der Hase mit dem Keks</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DEM.M.SG.NOM down-PASTP&gt;fall&lt;CIRC be.SG.PRS.IND</t>
+          <t>the.ART.DEF.M.SG.NOM hare.M.SG.NOM with the.ART.DEF.M.SG.DAT biscuit.M.SG.DAT</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>pferd das die kühe zieht</t>
+          <t>der hase ganz vorne</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>horse.SG REL.N.SG.NOM/ACC ART.DEF.PL.NOM/ACC cow-PL.NOM/ACC pull-.SG.PRS.IND</t>
+          <t>the.ART.DEF.M.SG.NOM hare.M.SG.NOM quite in-front</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>der die ente wascht</t>
+          <t>der vordere</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>DEM.M.SG.NOM ART.DEF.F.SG.NOM/ACC duck.F.SG.NOM/ACC wash-.SG.PRS.IND</t>
+          <t>the.ART.DEF.M.SG.NOM front.M.SG.NOM</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>der der ente die blume gibt</t>
+          <t>der hase</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DEM.M.SG.NOM ART.DEF.F.SG.DAT duck.F.SG.DAT ART.DEF.F.SG.NOM/ACC flower.F.SG.NOM/ACC give\PRS-.SG.IND</t>
+          <t>the.ART.DEF.M.SG.NOM hare.M.SG.NOM</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>die ziege die nicht springt</t>
+          <t>dass der hase blau wäre</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ART.DEF.F.SG.NOM/ACC goat.F.SG.NOM/ACC REL.F.SG.NOM/ACC NEG jump-.SG.PRS.IND</t>
+          <t>that the.ART.DEF.M.SG.NOM hare.M.SG.NOM blue be.SG.Past.Sub</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>das haus das in der mitte steht</t>
+          <t>der hase</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>ART.DEF.N.SG.NOM/ACC house.N.SG.NOM/ACC REL.N.SG.NOM/ACC in ART.DEF.F.SG.DAT middle.F.SG.DAT stay-.SG.PRS.IND</t>
+          <t>the.ART.DEF.M.SG.NOM hare.M.SG.NOM</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>der löwe die die kühe ziehen</t>
+          <t>der hase der hinfällt</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>ART.DEF.M.SG.NOM lion.M.SG.NOM REL.F.SG/PL.NOM/ACC ART.DEF.PL.NOM/ACC cow-PL.NOM/ACC pull-.PL.PRS.IND</t>
+          <t>the.ART.DEF.M.SG.NOM hare.M.SG.NOM the.DEM.M.SG.NOM fall.SG.PRS.IND</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>der hund der die schafe wascht</t>
+          <t>der Ball</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>ART.DEF.M.SG.NOM dog.M.SG.NOM REL.M.SG.NOM ART.DEF.PL.NOM/ACC sheep-PL.NOM/ACC wash-.SG.PRS.IND</t>
+          <t>the.ART.DEF.M.SG.NOM ball.M.SG.NOM</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>die frösche die die ente fangen</t>
+          <t>rollt</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>ART.DEF.PL.NOM/ACC frog-PL.NOM/ACC REL.PL.NOM/ACC ART.DEF.F:SG.NOM/ACC duck.F.SG.NOM/ACC catch-.PL.PRS.IND</t>
+          <t>roll</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>der die katzen ziehen den löwen</t>
+          <t>der Ball, der rollt</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DEM.M.SG.NOM ART.DEF.PL.NOM/ACC cat-PL.NOM/ACC pull-.PL.PRS.IND ART.DEF.M.SG.ACC lion.M.SG.ACC</t>
+          <t>the.ART.DEF.M.SG.NOM ball.M.SG.NOM  the.REL.M.SG.NOM roll.SG.PRS.IND</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>der frosch der an dem haus sitzt</t>
+          <t>das Pferd mit dem Zopf</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>ART.DEF.M.SG.NOM frog.M.SG.NOM REL.M.SG.NOM at ART.DEF.N.SG.DAT house.N.SG.DAT sit-.SG.PRS.IND</t>
+          <t>the.ART.DEF.N.SG.ACC horse.N.SG.NOM with the.ART.DEF.M.SG.DAT plait.M.SG.DAT</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>der frosch wo der frosch wach ist</t>
+          <t>das Pferd, das die Kühe zieht</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>ART.DEF.M.SG.NOM frog.M.SG.NOM where ART.DEF.M.SG.NOM frog.M.SG.NOM awake be.SG.PRS.IND</t>
+          <t>the.ART.DEF.N.SG.ACC horse.N.SG.ACC  the.REL.N.SG.NOM the.ART.DEF.F.PL.ACC cows.F.PL.ACC pull.SG.PRS.IND</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>den huhn der den maus den huhn den pfirsich gibt</t>
+          <t>da sitzen</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>ART.DEF.M.SG.ACC chicken.SG.NOM/ACC REL.M.SG.NOM ART.DEF.M.SG.ACC mouse.SG ART.DEF.M.SG.ACC chicken.SG.NOM/ACC ART.DEF.M.SG.ACC peach.M.SG.ACC give\PRS-.SG.IND</t>
+          <t>there sit</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>der den frosch der den dem huhn gibt</t>
+          <t>Ziege</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DEM.M.SG.NOM ART.DEF.M.SG.ACC frog.M.SG.ACC REL.M.SG.NOM DEM.M.SG.ACC ART.DEF.N.SG.DAT chicken.N.SG.DAT give\PRS-.SG.IND</t>
+          <t>goat.SG.NOM</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>wo die katze drauf hüpft</t>
+          <t>Baum</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>where ART.DEF.F.SG.NOM/ACC cat.F.SG.NOM/ACC on.top jump-.SG.PRS.IND</t>
+          <t>tree.M.SG.NOM</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>der huhn der den huhn zu dem hund wirft</t>
+          <t>da, wo die Ziege sitzt</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>ART.DEF.M.SG.NOM chicken.SG REL.M.SG.NOM ART.DEF.M.SG.ACC chicken.SG to ART.DEF.M.SG.DAT dog.M.SG.DAT throw\PRS-.SG.IND</t>
+          <t>there  where.INT the.ART.DEF.F.SG.NOM goat.F.SG.NOM sit.SG.PRS.IND</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>das das schaf fangt</t>
+          <t>die Frösche, die die Ente fangen</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>DEM/REL.N.SG.NOM/ACC ART.DEF.N.SG.NOM/ACC sheep.N.SG.NOM/ACC catch-.SG.PRS.IND</t>
+          <t>the.ART.DEF.M.PL.NOM frog.M.PL.NOM  the.REL.M.PL.NOM the.ART.DEF.F.SG.ACC duck.F.SG.ACC catch.PL.PRS.IND</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>das schaf die hunde fängt</t>
+          <t>die Hunde, die das Schaf gefangen genommen hat</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>ART.DEF.N.SG.NOM/ACC sheep.N.SG.NOM/ACC ART.DEF.PL.NOM/ACC dog-PL.NOM/ACC catch\PRS-.SG.IND</t>
+          <t>the.ART.DEF.M.PL.ACC dog.M.PL.ACC  the.REL.M.PL.NOM the.ART.DEF.N.SG.ACC sheep.N.SG.ACC caught take have.SG.PRS.IND</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>die ziegen die die katze schubsen</t>
+          <t>der Hund, wo das Huhn den Ball zum Hund wirft</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>ART.DEF.PL.NOM/ACC goat-PL.NOM/ACC REL.PL.NOM/ACC ART.DEF.F.SG.NOM/ACC cat.F.SG.NOM/ACC push-.PL.PRS.IND</t>
+          <t>the.ART.DEF.M.SG.NOM dog.M.SG.NOM  where.INT the.ART.DEF.N.SG.NOM chicken.N.SG.NOM the.ART.DEF.M.SG.ACC ball.M.SG.ACC to.M.SG.DAT dog.M.SG.DAT throw.SG.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>der Hund, der die Schafe wäscht</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.M.SG.NOM dog.M.SG.NOM  the.REL.M.SG.NOM the.ART.DEF.N.PL.ACC sheep.N.PL.ACC wash.SG.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>das Huhn, dem der Apfel zugeworfen wird</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.N.SG.NOM chicken.N.SG.ACC  the.REL.M.SG.DAT the.ART.DEF.M.SG.NOM apple.M.SG.NOM thrown-at become.SG.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>der Löwe, der die zwei Kühe zieht</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.M.SG.NOM lion.M.SG.NOM  the.REL.M.SG.NOM the.ART.DEF.F.PL.ACC two cows.F.PL.ACC pull.SG.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>das Huhn, das neben der Maus steht, und die Maus gibt dem Huhn die Pflaume</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.N.SG.NOM chicken.N.SG.NOM  the.REL.N.SG.NOM next-to the.ART.DEF.F.SG.DAT mouse.F.SG.DAT stand.SG.PRS.IND  and the.ART.DEF.F.SG.NOM mouse.F.SG.NOM give.SG.PRS.IND the.ART.DEF.M.SG.DAT chicken.M.SG.DAT the.ART.DEF.F.SG.ACC plum.F.SG.ACC</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>die Pferde, die das Schaf schubst ja die und ich vermute, die Pferde, die vom Stier oder Schaf geschubst werden</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.N.PL.ACC horse.N.PL.ACC  the.REL.N.PL.NOM the.ART.DEF.N.SG.ACC sheep.N.SG.ACC push.SG.PRS.IND yes the.DEM.F.SG.ACC and i.Prs.SG.NOM assume.SG.PRS.IND  the.ART.DEF.N.PL.ACC horse.N.PL.ACC  the.REL.N.PL.NOM from.M.SG.DAT bull.M.SG.DAT or sheep.N.SG.DAT push become.PL.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>der Frosch, der da sitzt unter dem Tisch</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.M.SG.NOM frog.M.SG.NOM  the.REL.M.SG.NOM there sit.SG.PRS.IND under the.ART.DEF.M.SG.DAT table.M.SG.DAT</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>der Tisch</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.M.SG.NOM table.M.SG.NOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>der, wo der Frosch drunter sitzt</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>the.DEM.M.SG.NOM  where.INT the.ART.DEF.M.SG.NOM frog.M.SG.NOM underneath sit.SG.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>die Ziegen, die die Katze schubsen</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.F.PL.ACC goat.F.PL.ACC  the.REL.F.PL.NOM the.ART.DEF.F.SG.ACC cat.F.SG.ACC push.PL.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>die Katze, die vor der Ente steht und die Ente gibt der Katze die Blume</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.F.SG.NOM cat.F.SG.NOM  the.REL.F.SG.NOM before the.ART.DEF.F.SG.DAT duck.F.SG.DAT stand.SG.PRS.IND and the.ART.DEF.F.SG.NOM duck.F.SG.NOM give.SG.PRS.IND the.ART.DEF.F.SG.DAT cat.F.SG.DAT the.ART.DEF.F.SG.ACC flower.F.SG.ACC</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>die Katze</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.F.SG.NOM cat.F.SG.NOM</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>der Frosch, der von den Enten gewaschen wird</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.M.SG.NOM frog.M.SG.NOM  the.REL.M.SG.NOM from the.ART.DEF.F.PL.DAT duck.F.PL.DAT wash become.SG.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>das Bett, auf dem die Katze springt</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.N.SG.ACC bed.N.SG.ACC  on the.REL.N.SG.DAT the.ART.DEF.F.SG.NOM cat.F.SG.NOM jump.SG.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>der Löwe, der von den Katzen gezogen wird</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.M.SG.NOM lion.M.SG.NOM  the.REL.M.SG.NOM from the.ART.DEF.F.PL.DAT cat.F.PL.DAT pull become.SG.PRS.IND</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>das Haus, auf dem das Schaf springt</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>the.ART.DEF.N.SG.ACC house.N.SG.ACC  on the.REL.N.SG.DAT the.ART.DEF.N.SG.NOM sheep.N.SG.NOM jump.SG.PRS.IND</t>
         </is>
       </c>
     </row>

</xml_diff>